<commit_message>
bug fix: location: others value
</commit_message>
<xml_diff>
--- a/reports/resume_extractor/resume_extraction_report.xlsx
+++ b/reports/resume_extractor/resume_extraction_report.xlsx
@@ -547,14 +547,14 @@
           <t>Mobile</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>1/5</t>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>0/5</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>20.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -564,14 +564,14 @@
           <t>Location</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>4/5</t>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>0/5</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -618,12 +618,12 @@
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>13/30</t>
+          <t>8/30</t>
         </is>
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>43.3%</t>
+          <t>26.7%</t>
         </is>
       </c>
     </row>
@@ -767,13 +767,17 @@
           <t>Others</t>
         </is>
       </c>
-      <c r="I2" s="9" t="inlineStr"/>
+      <c r="I2" s="10" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
       <c r="J2" t="n">
         <v>6.8</v>
       </c>
       <c r="K2" s="9" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -836,7 +840,7 @@
       </c>
       <c r="K3" s="9" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -879,9 +883,9 @@
       <c r="F4" t="n">
         <v>8373992286</v>
       </c>
-      <c r="G4" s="9" t="inlineStr">
-        <is>
-          <t>9873392286</t>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>8373992286</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -889,7 +893,11 @@
           <t>Others</t>
         </is>
       </c>
-      <c r="I4" s="9" t="inlineStr"/>
+      <c r="I4" s="10" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
       <c r="J4" t="n">
         <v>14.7</v>
       </c>
@@ -944,7 +952,11 @@
           <t>Others</t>
         </is>
       </c>
-      <c r="I5" s="9" t="inlineStr"/>
+      <c r="I5" s="10" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
       <c r="J5" t="n">
         <v>6</v>
       </c>
@@ -1003,13 +1015,17 @@
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="I6" s="9" t="inlineStr"/>
+      <c r="I6" s="10" t="inlineStr">
+        <is>
+          <t>bengaluru</t>
+        </is>
+      </c>
       <c r="J6" t="n">
         <v>3.4</v>
       </c>
       <c r="K6" s="9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">

</xml_diff>

<commit_message>
bug fix: experince comparison
</commit_message>
<xml_diff>
--- a/reports/resume_extractor/resume_extraction_report.xlsx
+++ b/reports/resume_extractor/resume_extraction_report.xlsx
@@ -530,14 +530,14 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>0/5</t>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>1/5</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -547,14 +547,14 @@
           <t>Mobile</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>0/5</t>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>1/5</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -583,12 +583,12 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>4/5</t>
+          <t>1/5</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -618,12 +618,12 @@
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>8/30</t>
+          <t>7/30</t>
         </is>
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>26.7%</t>
+          <t>23.3%</t>
         </is>
       </c>
     </row>
@@ -775,9 +775,9 @@
       <c r="J2" t="n">
         <v>6.8</v>
       </c>
-      <c r="K2" s="9" t="inlineStr">
-        <is>
-          <t>7.7</t>
+      <c r="K2" s="10" t="inlineStr">
+        <is>
+          <t>6.6</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -875,17 +875,17 @@
           <t>vibhormalik05@gmail.com</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
-        <is>
-          <t>vibhormalik05@gmail.com</t>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>malikvibhor@linkedin.com</t>
         </is>
       </c>
       <c r="F4" t="n">
         <v>8373992286</v>
       </c>
-      <c r="G4" s="10" t="inlineStr">
-        <is>
-          <t>8373992286</t>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
+          <t>9873392286</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -960,7 +960,7 @@
       <c r="J5" t="n">
         <v>6</v>
       </c>
-      <c r="K5" s="9" t="inlineStr">
+      <c r="K5" s="10" t="inlineStr">
         <is>
           <t>5.11</t>
         </is>
@@ -1023,7 +1023,7 @@
       <c r="J6" t="n">
         <v>3.4</v>
       </c>
-      <c r="K6" s="9" t="inlineStr">
+      <c r="K6" s="10" t="inlineStr">
         <is>
           <t>3.0</t>
         </is>

</xml_diff>